<commit_message>
add class 03 conditionals
</commit_message>
<xml_diff>
--- a/1-Excel/class-01-math-operations.xlsx
+++ b/1-Excel/class-01-math-operations.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40cbc61c02823304/Área de Trabalho/Emanuel/Data-Analyst-Course/1-Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="11_AD4D361C20488DEA4E38A0DDDC5C55145ADEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D59D7C69-B6D7-4AB1-9632-C78F31DCF761}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="11_AD4D361C20488DEA4E38A0DDDC5C55145ADEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AB59162-3AD1-4DAC-B05F-09EF3DA100E9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="OPERAÇÕES" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>PREÇO</t>
   </si>
@@ -104,13 +104,19 @@
     <t>DIVISÃO</t>
   </si>
   <si>
-    <t>FUNÇÕES</t>
-  </si>
-  <si>
     <t>MÉDIA</t>
   </si>
   <si>
     <t>TABELA DE COMPRAS</t>
+  </si>
+  <si>
+    <t>MÍNIMO</t>
+  </si>
+  <si>
+    <t>MÁXIMO</t>
+  </si>
+  <si>
+    <t>FUNÇÕES MATEMÁTICAS</t>
   </si>
 </sst>
 </file>
@@ -205,7 +211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -230,6 +236,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -246,6 +254,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -514,7 +526,7 @@
   <dimension ref="B2:K14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -523,12 +535,12 @@
     <col min="3" max="4" width="8.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="1.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -547,8 +559,8 @@
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
-        <v>22</v>
+      <c r="J3" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.35">
@@ -565,14 +577,18 @@
         <f>C4*D4</f>
         <v>6</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="11" t="s">
         <v>14</v>
+      </c>
+      <c r="K4" s="7">
+        <f>SUM(E4:E13)</f>
+        <v>146.13</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.35">
@@ -589,13 +605,13 @@
         <f t="shared" ref="E5:E13" si="0">C5*D5</f>
         <v>7.0500000000000007</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="11" t="s">
         <v>12</v>
       </c>
       <c r="K5">
@@ -617,14 +633,14 @@
         <f t="shared" si="0"/>
         <v>4.2</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J6" t="s">
-        <v>23</v>
+      <c r="J6" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="K6" s="7">
         <f>AVERAGE(E4:E13)</f>
@@ -645,11 +661,18 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="10" t="s">
         <v>21</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="7">
+        <f>MIN(E4:E13)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
@@ -665,6 +688,13 @@
       <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>34.019999999999996</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="7">
+        <f>MAX(E4:E13)</f>
+        <v>69.23</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.35">

</xml_diff>